<commit_message>
tri categorie dans gérer articles et ajout mail pour nouvelle campagne
</commit_message>
<xml_diff>
--- a/burndown.xlsx
+++ b/burndown.xlsx
@@ -1394,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49:R49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>